<commit_message>
feat: remove categories from product schema
</commit_message>
<xml_diff>
--- a/ai_service/backend/core/tests/core/models/data_test.xlsx
+++ b/ai_service/backend/core/tests/core/models/data_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Product_Name</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Categories</t>
   </si>
   <si>
     <t>Category_tier_one</t>
@@ -50,9 +47,6 @@
     <t>Quần Short Kaki thiết kế eo thun, thoải mái vòng bụng, from slim vừa vặn tôn dáng và không quá ôm sát, tạo sự thoải mái cho người mặc. Lót trong may hoàn thiện sắc nét, dây kéo YKK bền bỉ trong quá trình sử dụng. Quần short kaki dễ dàng phối với áo thun, polo đa dạng trong từng phong cách. Chất liệu vải kaki co giãn, bền màu, vải siêu mát và ít nhăn khi mặc.</t>
   </si>
   <si>
-    <t>quần short, quần short kaki, kaki, be, việt nam, nam, m, co giãn, bền màu, slimfit, eo thun</t>
-  </si>
-  <si>
     <t>thời trang nam</t>
   </si>
   <si>
@@ -76,9 +70,6 @@
     <t>https://product.hstatic.net/1000096703/product/1_3a7bc8dc92f14b2990adf620965535de_master.jpg</t>
   </si>
   <si>
-    <t>quần short, quần short kaki, kaki, be, việt nam, nam, s, m, l, xl, xxl, co giãn, bền màu, ít nhăn, thoải mái, tôn dáng</t>
-  </si>
-  <si>
     <t>Quần Short Kaki Lưng Thun, Dây Kéo QSL0061
 SKU: QSL006129XT</t>
   </si>
@@ -89,9 +80,6 @@
     <t>Quần Short Kaki Nam lưng thun kết hợp dây kéo. Chất vải kaki mịn và mát. Form trên gối, vừa vặn. Chất liệu co co giãn, mặc cực kì thoải mái. Thử ngay sản phẩm này của Kenta nhé.</t>
   </si>
   <si>
-    <t>quần short, quần short nam, kaki, kem, việt nam, m, l, xl, xxl, thoải mái, năng động</t>
-  </si>
-  <si>
     <t>Quần Short Kaki Nam QSK0065
 SKU: QSK006529DE</t>
   </si>
@@ -102,9 +90,6 @@
     <t>Quần Short Kaki nam năng động trẻ trung, from slim vừa vặn tôn dáng và không quá ôm sát, tạo sự thoải mái cho người mặc. Lót trong may hoàn thiện sắc nét, dây kéo YKK bền bỉ trong quá trình sử dụng. Quần short kaki dễ dàng phối với áo thun, polo đa dạng trong từng phong cách. Chất liệu vải kaki co giãn, bền màu, vải siêu mát và ít nhăn khi mặc.</t>
   </si>
   <si>
-    <t>quần short, quần short nam, kaki, be, việt nam, m, l, xl, xxl, năng động, trẻ trung, thoải mái, bền màu, ít nhăn</t>
-  </si>
-  <si>
     <t>Quần Short Kaki Nam QSK0065
 SKU: QSK006529XĐ</t>
   </si>
@@ -112,17 +97,11 @@
     <t>https://product.hstatic.net/1000096703/product/1_7a4b5f32dc2b4ec3a0e389c9020dcada_master.jpg</t>
   </si>
   <si>
-    <t>quần short, quần short nam, kaki, be, việt nam, s, m, l, xl, xxl, năng động, trẻ trung, thoải mái, bền màu, ít nhăn</t>
-  </si>
-  <si>
     <t>Quần Short Kaki Nam QSK0065
 SKU: QSK006529XA</t>
   </si>
   <si>
     <t>https://product.hstatic.net/1000096703/product/1_62d45f243b3e412d827fee92450c1dfb_master.jpg</t>
-  </si>
-  <si>
-    <t>quần short, quần short nam, kaki, xanh navy, việt nam, m, l, xl, xxl, năng động, trẻ trung, thoải mái, tôn dáng, co giãn, bền màu, ít nhăn</t>
   </si>
   <si>
     <t>Quần Short Kaki Nam QSK0065
@@ -530,7 +509,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -540,10 +519,9 @@
     <col min="2" max="2" style="5" width="51.14785714285715" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="5" width="34.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="55.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="15.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -568,242 +546,212 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="31.5">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4">
+        <v>220000</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
-        <v>220000</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="31.5">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4">
         <v>220000</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>220000</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="31.5">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4">
         <v>220000</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="31.5">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4">
         <v>220000</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="31.5">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4">
         <v>220000</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="31.5">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C8" s="4">
         <v>220000</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="31.5">
       <c r="A9" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4">
         <v>220000</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="31.5">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C10" s="4">
         <v>220000</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>